<commit_message>
Added ifs to user's id
</commit_message>
<xml_diff>
--- a/PatientCare360/Excel/Patients.xlsx
+++ b/PatientCare360/Excel/Patients.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -179,6 +179,9 @@
 Diagnoses Iron deficiency
 Treatment: Required to take two pills of 10 mg of B12 a day for a month
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
   </si>
 </sst>
 </file>
@@ -793,6 +796,72 @@
       <c r="U4" t="s">
         <v>48</v>
       </c>
+      <c r="V4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed label pf Patient Questioner to Questionnaire
</commit_message>
<xml_diff>
--- a/PatientCare360/Excel/Patients.xlsx
+++ b/PatientCare360/Excel/Patients.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="63">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -236,6 +236,12 @@
 Diagnoses Malnutrition
 Treatment: Ask for an appointment of a nutritionist
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5783522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90</t>
   </si>
 </sst>
 </file>
@@ -1112,6 +1118,328 @@
       <c r="U8" t="s">
         <v>36</v>
       </c>
+      <c r="V8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" t="s">
+        <v>35</v>
+      </c>
+      <c r="T9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" t="s">
+        <v>36</v>
+      </c>
+      <c r="V9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" t="s">
+        <v>34</v>
+      </c>
+      <c r="S10" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10"/>
+      <c r="V10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" t="s">
+        <v>36</v>
+      </c>
+      <c r="V11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" t="s">
+        <v>35</v>
+      </c>
+      <c r="T12" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12"/>
+      <c r="V12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" t="s">
+        <v>34</v>
+      </c>
+      <c r="S13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>